<commit_message>
curso completo de php
</commit_message>
<xml_diff>
--- a/00soportes/Tiempos.xlsx
+++ b/00soportes/Tiempos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cvpetrix2022\00soportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A03966-B565-4A1A-9B80-B4D7B420A35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AE3519-96C5-452B-8456-D9D0FAFDFF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E9525E9-3A51-4A38-A83E-5673FF3CE17A}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="116">
   <si>
     <t>Fecha</t>
   </si>
@@ -390,6 +390,9 @@
   <si>
     <t>https://campus-ademass.com/curso/4</t>
   </si>
+  <si>
+    <t>PHP</t>
+  </si>
 </sst>
 </file>
 
@@ -627,8 +630,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D41BB900-8286-45A6-904E-18FDD4B4DC1E}" name="Tabla2" displayName="Tabla2" ref="A1:S324" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A1:S324" xr:uid="{D41BB900-8286-45A6-904E-18FDD4B4DC1E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D41BB900-8286-45A6-904E-18FDD4B4DC1E}" name="Tabla2" displayName="Tabla2" ref="A1:S332" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A1:S332" xr:uid="{D41BB900-8286-45A6-904E-18FDD4B4DC1E}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="PHP"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="18">
       <filters>
         <filter val="2024"/>
@@ -665,10 +673,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F07769A-B222-4F9A-993F-A5C63DFC99D9}" name="Tabla1" displayName="Tabla1" ref="A1:A16" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:A16" xr:uid="{4F07769A-B222-4F9A-993F-A5C63DFC99D9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A16">
-    <sortCondition ref="A1:A16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F07769A-B222-4F9A-993F-A5C63DFC99D9}" name="Tabla1" displayName="Tabla1" ref="A1:A17" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:A17" xr:uid="{4F07769A-B222-4F9A-993F-A5C63DFC99D9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A17">
+    <sortCondition ref="A1:A17"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{AAEDA63C-5001-4ADA-84DC-0BDF6170A151}" name="Tecnologías"/>
@@ -974,13 +982,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D3FF4A-8960-4190-B595-1BF8B3DB0A5F}">
-  <dimension ref="A1:X324"/>
+  <dimension ref="A1:X338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D313" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F327" sqref="F327"/>
+      <selection pane="bottomRight" activeCell="C325" sqref="C325:C332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,15 +1066,15 @@
       </c>
       <c r="V1" s="15">
         <f>Resumen!D2</f>
-        <v>42.031413612565444</v>
+        <v>44.126903553299492</v>
       </c>
       <c r="W1" s="17">
         <f>Resumen!D11</f>
-        <v>0.73114754098360657</v>
+        <v>0.79171220400728592</v>
       </c>
       <c r="X1" s="19">
         <f>Resumen!D7+Resumen!F10</f>
-        <v>45559</v>
+        <v>45581</v>
       </c>
     </row>
     <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
@@ -5255,7 +5263,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>45293</v>
       </c>
@@ -5296,7 +5304,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>45294</v>
       </c>
@@ -5333,7 +5341,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>45295</v>
       </c>
@@ -5374,7 +5382,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>45296</v>
       </c>
@@ -5419,7 +5427,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>45297</v>
       </c>
@@ -5466,7 +5474,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>45298</v>
       </c>
@@ -5511,7 +5519,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>45299</v>
       </c>
@@ -5548,7 +5556,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>45300</v>
       </c>
@@ -5585,7 +5593,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>45301</v>
       </c>
@@ -5622,7 +5630,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>45302</v>
       </c>
@@ -5657,7 +5665,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>45303</v>
       </c>
@@ -5696,7 +5704,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>45306</v>
       </c>
@@ -5731,7 +5739,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>45307</v>
       </c>
@@ -5768,7 +5776,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>45308</v>
       </c>
@@ -5803,7 +5811,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>45309</v>
       </c>
@@ -5844,7 +5852,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>45313</v>
       </c>
@@ -5879,7 +5887,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>45314</v>
       </c>
@@ -5912,7 +5920,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>45315</v>
       </c>
@@ -5947,7 +5955,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>45316</v>
       </c>
@@ -5982,7 +5990,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>45317</v>
       </c>
@@ -6017,7 +6025,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>45318</v>
       </c>
@@ -6050,7 +6058,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>45319</v>
       </c>
@@ -6085,7 +6093,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>45320</v>
       </c>
@@ -6120,7 +6128,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>45320</v>
       </c>
@@ -6153,7 +6161,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>45321</v>
       </c>
@@ -6186,7 +6194,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>45321</v>
       </c>
@@ -6220,7 +6228,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>45322</v>
       </c>
@@ -6255,7 +6263,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>45322</v>
       </c>
@@ -6289,7 +6297,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>45323</v>
       </c>
@@ -6324,7 +6332,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>45323</v>
       </c>
@@ -6357,7 +6365,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>45324</v>
       </c>
@@ -6390,7 +6398,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>45324</v>
       </c>
@@ -6424,7 +6432,7 @@
       </c>
       <c r="U134" s="3"/>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>45326</v>
       </c>
@@ -6459,7 +6467,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>45327</v>
       </c>
@@ -6494,7 +6502,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>45328</v>
       </c>
@@ -6527,7 +6535,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>45328</v>
       </c>
@@ -6560,7 +6568,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>45329</v>
       </c>
@@ -6593,7 +6601,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>45329</v>
       </c>
@@ -6628,7 +6636,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>45330</v>
       </c>
@@ -6663,7 +6671,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>45330</v>
       </c>
@@ -6696,7 +6704,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>45331</v>
       </c>
@@ -6731,7 +6739,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>45334</v>
       </c>
@@ -6764,7 +6772,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>45334</v>
       </c>
@@ -6797,7 +6805,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>45335</v>
       </c>
@@ -6830,7 +6838,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>45335</v>
       </c>
@@ -6863,7 +6871,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>45336</v>
       </c>
@@ -6896,7 +6904,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>45336</v>
       </c>
@@ -6929,7 +6937,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>45337</v>
       </c>
@@ -6964,7 +6972,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>45337</v>
       </c>
@@ -6997,7 +7005,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>45338</v>
       </c>
@@ -7030,7 +7038,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>45338</v>
       </c>
@@ -7063,7 +7071,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>45339</v>
       </c>
@@ -7096,7 +7104,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>45339</v>
       </c>
@@ -7129,7 +7137,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>45340</v>
       </c>
@@ -7164,7 +7172,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>45340</v>
       </c>
@@ -7197,7 +7205,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>45341</v>
       </c>
@@ -7232,7 +7240,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>45341</v>
       </c>
@@ -7265,7 +7273,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>45342</v>
       </c>
@@ -7300,7 +7308,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>45342</v>
       </c>
@@ -7333,7 +7341,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>45343</v>
       </c>
@@ -7368,7 +7376,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>45343</v>
       </c>
@@ -7401,7 +7409,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>45344</v>
       </c>
@@ -7434,7 +7442,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>45344</v>
       </c>
@@ -7467,7 +7475,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>45345</v>
       </c>
@@ -7508,7 +7516,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>45345</v>
       </c>
@@ -7541,7 +7549,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>45346</v>
       </c>
@@ -7586,7 +7594,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>45346</v>
       </c>
@@ -7619,7 +7627,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>45347</v>
       </c>
@@ -7664,7 +7672,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>45347</v>
       </c>
@@ -7697,7 +7705,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>45348</v>
       </c>
@@ -7736,7 +7744,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>45348</v>
       </c>
@@ -7769,7 +7777,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>45349</v>
       </c>
@@ -7810,7 +7818,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>45349</v>
       </c>
@@ -7848,7 +7856,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>45350</v>
       </c>
@@ -7887,7 +7895,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>45350</v>
       </c>
@@ -7920,7 +7928,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>45351</v>
       </c>
@@ -7959,7 +7967,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>45351</v>
       </c>
@@ -7992,7 +8000,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>45352</v>
       </c>
@@ -8037,7 +8045,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>45352</v>
       </c>
@@ -8070,7 +8078,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>45353</v>
       </c>
@@ -8115,7 +8123,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>45353</v>
       </c>
@@ -8148,7 +8156,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>45354</v>
       </c>
@@ -8181,7 +8189,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>45354</v>
       </c>
@@ -8215,7 +8223,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>45355</v>
       </c>
@@ -8248,7 +8256,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>45355</v>
       </c>
@@ -8281,7 +8289,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>45356</v>
       </c>
@@ -8322,7 +8330,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>45356</v>
       </c>
@@ -8355,7 +8363,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>45357</v>
       </c>
@@ -8394,7 +8402,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>45357</v>
       </c>
@@ -8427,7 +8435,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>45358</v>
       </c>
@@ -8466,7 +8474,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>45358</v>
       </c>
@@ -8499,7 +8507,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>45359</v>
       </c>
@@ -8534,7 +8542,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>45359</v>
       </c>
@@ -8567,7 +8575,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>45360</v>
       </c>
@@ -8606,7 +8614,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>45361</v>
       </c>
@@ -8645,7 +8653,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>45362</v>
       </c>
@@ -8684,7 +8692,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>45362</v>
       </c>
@@ -8721,7 +8729,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>45363</v>
       </c>
@@ -8764,7 +8772,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>45363</v>
       </c>
@@ -8797,7 +8805,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>45364</v>
       </c>
@@ -8838,7 +8846,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>45365</v>
       </c>
@@ -8877,7 +8885,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>45366</v>
       </c>
@@ -8914,7 +8922,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>45366</v>
       </c>
@@ -8947,7 +8955,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>45367</v>
       </c>
@@ -8984,7 +8992,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>45368</v>
       </c>
@@ -9025,7 +9033,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>45369</v>
       </c>
@@ -9058,7 +9066,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>45369</v>
       </c>
@@ -9091,7 +9099,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>45370</v>
       </c>
@@ -9134,7 +9142,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>45370</v>
       </c>
@@ -9167,7 +9175,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>45371</v>
       </c>
@@ -9200,7 +9208,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>45371</v>
       </c>
@@ -9233,7 +9241,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>45372</v>
       </c>
@@ -9266,7 +9274,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>45372</v>
       </c>
@@ -9299,7 +9307,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>45373</v>
       </c>
@@ -9332,7 +9340,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>45373</v>
       </c>
@@ -9365,7 +9373,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>45373</v>
       </c>
@@ -9398,7 +9406,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>45375</v>
       </c>
@@ -9431,7 +9439,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>45376</v>
       </c>
@@ -9464,7 +9472,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>45377</v>
       </c>
@@ -9505,7 +9513,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>45377</v>
       </c>
@@ -9538,7 +9546,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>45378</v>
       </c>
@@ -9575,7 +9583,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>45383</v>
       </c>
@@ -9610,7 +9618,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>45383</v>
       </c>
@@ -9643,7 +9651,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>45384</v>
       </c>
@@ -9680,7 +9688,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>45384</v>
       </c>
@@ -9713,7 +9721,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>45385</v>
       </c>
@@ -9750,7 +9758,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>45385</v>
       </c>
@@ -9783,7 +9791,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>45386</v>
       </c>
@@ -9820,7 +9828,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>45386</v>
       </c>
@@ -9853,7 +9861,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>45387</v>
       </c>
@@ -9896,7 +9904,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>45387</v>
       </c>
@@ -9929,7 +9937,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>45390</v>
       </c>
@@ -9962,7 +9970,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>45391</v>
       </c>
@@ -9995,7 +10003,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>45392</v>
       </c>
@@ -10028,7 +10036,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>45393</v>
       </c>
@@ -10061,7 +10069,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>45394</v>
       </c>
@@ -10094,7 +10102,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>45394</v>
       </c>
@@ -10127,7 +10135,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>45395</v>
       </c>
@@ -10162,7 +10170,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>45396</v>
       </c>
@@ -10197,7 +10205,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>45397</v>
       </c>
@@ -10230,7 +10238,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>45398</v>
       </c>
@@ -10263,7 +10271,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>45399</v>
       </c>
@@ -10298,7 +10306,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>45400</v>
       </c>
@@ -10335,7 +10343,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>45401</v>
       </c>
@@ -10368,7 +10376,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>45404</v>
       </c>
@@ -10405,7 +10413,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>45405</v>
       </c>
@@ -10446,7 +10454,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>45406</v>
       </c>
@@ -10487,7 +10495,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>45407</v>
       </c>
@@ -10522,7 +10530,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>45408</v>
       </c>
@@ -10559,7 +10567,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>45410</v>
       </c>
@@ -10594,7 +10602,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>45411</v>
       </c>
@@ -10633,7 +10641,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>45412</v>
       </c>
@@ -10670,7 +10678,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>45414</v>
       </c>
@@ -10711,7 +10719,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>45415</v>
       </c>
@@ -10744,7 +10752,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>45418</v>
       </c>
@@ -10779,7 +10787,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>45419</v>
       </c>
@@ -10824,7 +10832,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>45420</v>
       </c>
@@ -10859,7 +10867,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>45421</v>
       </c>
@@ -10898,7 +10906,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>45422</v>
       </c>
@@ -10941,7 +10949,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>45423</v>
       </c>
@@ -10974,7 +10982,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>45424</v>
       </c>
@@ -11009,7 +11017,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>45425</v>
       </c>
@@ -11052,7 +11060,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>45425</v>
       </c>
@@ -11089,7 +11097,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>45426</v>
       </c>
@@ -11126,7 +11134,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>45426</v>
       </c>
@@ -11159,7 +11167,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>45427</v>
       </c>
@@ -11198,7 +11206,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>45427</v>
       </c>
@@ -11231,7 +11239,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>45428</v>
       </c>
@@ -11264,7 +11272,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>45429</v>
       </c>
@@ -11301,7 +11309,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>45429</v>
       </c>
@@ -11336,7 +11344,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>45430</v>
       </c>
@@ -11373,7 +11381,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>45432</v>
       </c>
@@ -11406,7 +11414,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>45433</v>
       </c>
@@ -11439,7 +11447,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>45434</v>
       </c>
@@ -11472,7 +11480,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>45435</v>
       </c>
@@ -11505,7 +11513,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>45436</v>
       </c>
@@ -11546,7 +11554,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>45439</v>
       </c>
@@ -11587,7 +11595,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>45440</v>
       </c>
@@ -11620,7 +11628,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>45441</v>
       </c>
@@ -11653,7 +11661,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>45442</v>
       </c>
@@ -11686,7 +11694,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>45442</v>
       </c>
@@ -11719,7 +11727,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>45443</v>
       </c>
@@ -11752,7 +11760,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>45443</v>
       </c>
@@ -11785,7 +11793,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>45446</v>
       </c>
@@ -11818,7 +11826,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>45447</v>
       </c>
@@ -11851,7 +11859,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <v>45452</v>
       </c>
@@ -11884,7 +11892,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>45453</v>
       </c>
@@ -11919,7 +11927,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>45454</v>
       </c>
@@ -11968,7 +11976,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>45455</v>
       </c>
@@ -12019,7 +12027,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>45456</v>
       </c>
@@ -12060,7 +12068,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>45457</v>
       </c>
@@ -12105,7 +12113,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>45460</v>
       </c>
@@ -12138,7 +12146,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>45461</v>
       </c>
@@ -12171,7 +12179,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>45462</v>
       </c>
@@ -12204,7 +12212,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>45463</v>
       </c>
@@ -12237,7 +12245,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>45464</v>
       </c>
@@ -12270,7 +12278,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>45467</v>
       </c>
@@ -12303,7 +12311,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>45467</v>
       </c>
@@ -12336,7 +12344,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>45468</v>
       </c>
@@ -12369,7 +12377,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>45468</v>
       </c>
@@ -12402,7 +12410,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>45469</v>
       </c>
@@ -12435,7 +12443,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>45471</v>
       </c>
@@ -12468,7 +12476,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>45472</v>
       </c>
@@ -12502,7 +12510,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>45472</v>
       </c>
@@ -12535,7 +12543,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>45473</v>
       </c>
@@ -12568,7 +12576,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>45475</v>
       </c>
@@ -12601,7 +12609,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <v>45476</v>
       </c>
@@ -12634,7 +12642,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <v>45477</v>
       </c>
@@ -12667,7 +12675,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>45477</v>
       </c>
@@ -12700,7 +12708,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <v>45478</v>
       </c>
@@ -12733,7 +12741,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>45478</v>
       </c>
@@ -12766,7 +12774,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>45479</v>
       </c>
@@ -12799,7 +12807,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>45479</v>
       </c>
@@ -12832,7 +12840,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>45479</v>
       </c>
@@ -12865,7 +12873,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>45479</v>
       </c>
@@ -12898,7 +12906,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>45480</v>
       </c>
@@ -12935,7 +12943,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>45481</v>
       </c>
@@ -12943,7 +12951,7 @@
         <v>25</v>
       </c>
       <c r="C319" s="4">
-        <f>SUM(D319:R319)</f>
+        <f t="shared" ref="C319:C324" si="51">SUM(D319:R319)</f>
         <v>55</v>
       </c>
       <c r="D319" s="3">
@@ -12968,7 +12976,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>45481</v>
       </c>
@@ -12976,7 +12984,7 @@
         <v>109</v>
       </c>
       <c r="C320" s="4">
-        <f>SUM(D320:R320)</f>
+        <f t="shared" si="51"/>
         <v>6</v>
       </c>
       <c r="D320" s="3">
@@ -13001,7 +13009,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="321" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>45481</v>
       </c>
@@ -13009,7 +13017,7 @@
         <v>108</v>
       </c>
       <c r="C321" s="4">
-        <f>SUM(D321:R321)</f>
+        <f t="shared" si="51"/>
         <v>9</v>
       </c>
       <c r="D321" s="3">
@@ -13034,7 +13042,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="322" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>45482</v>
       </c>
@@ -13042,7 +13050,7 @@
         <v>25</v>
       </c>
       <c r="C322" s="4">
-        <f>SUM(D322:R322)</f>
+        <f t="shared" si="51"/>
         <v>48</v>
       </c>
       <c r="D322" s="3">
@@ -13067,7 +13075,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="323" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>45482</v>
       </c>
@@ -13075,7 +13083,7 @@
         <v>7</v>
       </c>
       <c r="C323" s="4">
-        <f>SUM(D323:R323)</f>
+        <f t="shared" si="51"/>
         <v>24</v>
       </c>
       <c r="D323" s="3">
@@ -13102,7 +13110,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="324" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>45482</v>
       </c>
@@ -13110,7 +13118,7 @@
         <v>109</v>
       </c>
       <c r="C324" s="4">
-        <f>SUM(D324:R324)</f>
+        <f t="shared" si="51"/>
         <v>17</v>
       </c>
       <c r="D324" s="3">
@@ -13134,6 +13142,363 @@
         <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
         <v>2024</v>
       </c>
+    </row>
+    <row r="325" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A325" s="1">
+        <v>45482</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C325" s="4">
+        <f t="shared" ref="C325:C330" si="52">SUM(D325:R325)</f>
+        <v>153</v>
+      </c>
+      <c r="D325" s="3">
+        <v>3</v>
+      </c>
+      <c r="E325" s="3">
+        <v>22</v>
+      </c>
+      <c r="F325" s="3">
+        <v>17</v>
+      </c>
+      <c r="G325" s="3">
+        <v>8</v>
+      </c>
+      <c r="H325" s="3">
+        <v>5</v>
+      </c>
+      <c r="I325" s="3">
+        <v>13</v>
+      </c>
+      <c r="J325" s="3">
+        <v>9</v>
+      </c>
+      <c r="K325" s="3">
+        <v>23</v>
+      </c>
+      <c r="L325" s="3">
+        <v>9</v>
+      </c>
+      <c r="M325" s="3">
+        <v>14</v>
+      </c>
+      <c r="N325" s="3">
+        <v>8</v>
+      </c>
+      <c r="O325" s="3">
+        <v>7</v>
+      </c>
+      <c r="P325" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q325" s="3"/>
+      <c r="R325" s="3"/>
+      <c r="S325" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="326" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A326" s="1">
+        <v>45483</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C326" s="4">
+        <f t="shared" si="52"/>
+        <v>159</v>
+      </c>
+      <c r="D326" s="3">
+        <v>14</v>
+      </c>
+      <c r="E326" s="3">
+        <v>9</v>
+      </c>
+      <c r="F326" s="3">
+        <v>8</v>
+      </c>
+      <c r="G326" s="3">
+        <v>12</v>
+      </c>
+      <c r="H326" s="3">
+        <v>6</v>
+      </c>
+      <c r="I326" s="3">
+        <v>12</v>
+      </c>
+      <c r="J326" s="3">
+        <v>6</v>
+      </c>
+      <c r="K326" s="3">
+        <v>9</v>
+      </c>
+      <c r="L326" s="3">
+        <v>10</v>
+      </c>
+      <c r="M326" s="3">
+        <v>12</v>
+      </c>
+      <c r="N326" s="3">
+        <v>9</v>
+      </c>
+      <c r="O326" s="3">
+        <v>10</v>
+      </c>
+      <c r="P326" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q326" s="3">
+        <v>16</v>
+      </c>
+      <c r="R326" s="3">
+        <v>11</v>
+      </c>
+      <c r="S326" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="327" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A327" s="1">
+        <v>45483</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C327" s="4">
+        <f t="shared" si="52"/>
+        <v>12</v>
+      </c>
+      <c r="D327" s="3">
+        <v>12</v>
+      </c>
+      <c r="E327" s="3"/>
+      <c r="F327" s="3"/>
+      <c r="G327" s="3"/>
+      <c r="H327" s="3"/>
+      <c r="I327" s="3"/>
+      <c r="J327" s="3"/>
+      <c r="K327" s="3"/>
+      <c r="L327" s="3"/>
+      <c r="M327" s="3"/>
+      <c r="N327" s="3"/>
+      <c r="O327" s="3"/>
+      <c r="P327" s="3"/>
+      <c r="Q327" s="3"/>
+      <c r="R327" s="3"/>
+      <c r="S327" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="328" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A328" s="1">
+        <v>45484</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C328" s="4">
+        <f t="shared" si="52"/>
+        <v>100</v>
+      </c>
+      <c r="D328" s="3">
+        <v>15</v>
+      </c>
+      <c r="E328" s="3">
+        <v>14</v>
+      </c>
+      <c r="F328" s="3">
+        <v>18</v>
+      </c>
+      <c r="G328" s="3">
+        <v>15</v>
+      </c>
+      <c r="H328" s="3">
+        <v>7</v>
+      </c>
+      <c r="I328" s="3">
+        <v>4</v>
+      </c>
+      <c r="J328" s="3">
+        <v>5</v>
+      </c>
+      <c r="K328" s="3">
+        <v>10</v>
+      </c>
+      <c r="L328" s="3">
+        <v>12</v>
+      </c>
+      <c r="M328" s="3"/>
+      <c r="N328" s="3"/>
+      <c r="O328" s="3"/>
+      <c r="P328" s="3"/>
+      <c r="Q328" s="3"/>
+      <c r="R328" s="3"/>
+      <c r="S328" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="329" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A329" s="1">
+        <v>45484</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C329" s="4">
+        <f t="shared" si="52"/>
+        <v>10</v>
+      </c>
+      <c r="D329" s="3">
+        <v>10</v>
+      </c>
+      <c r="E329" s="3"/>
+      <c r="F329" s="3"/>
+      <c r="G329" s="3"/>
+      <c r="H329" s="3"/>
+      <c r="I329" s="3"/>
+      <c r="J329" s="3"/>
+      <c r="K329" s="3"/>
+      <c r="L329" s="3"/>
+      <c r="M329" s="3"/>
+      <c r="N329" s="3"/>
+      <c r="O329" s="3"/>
+      <c r="P329" s="3"/>
+      <c r="Q329" s="3"/>
+      <c r="R329" s="3"/>
+      <c r="S329" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="330" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A330" s="1">
+        <v>45485</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C330" s="4">
+        <f t="shared" si="52"/>
+        <v>77</v>
+      </c>
+      <c r="D330" s="3">
+        <v>11</v>
+      </c>
+      <c r="E330" s="3">
+        <v>16</v>
+      </c>
+      <c r="F330" s="3">
+        <v>20</v>
+      </c>
+      <c r="G330" s="3">
+        <v>17</v>
+      </c>
+      <c r="H330" s="3">
+        <v>13</v>
+      </c>
+      <c r="I330" s="3"/>
+      <c r="J330" s="3"/>
+      <c r="K330" s="3"/>
+      <c r="L330" s="3"/>
+      <c r="M330" s="3"/>
+      <c r="N330" s="3"/>
+      <c r="O330" s="3"/>
+      <c r="P330" s="3"/>
+      <c r="Q330" s="3"/>
+      <c r="R330" s="3"/>
+      <c r="S330" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="331" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A331" s="1">
+        <v>45487</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C331" s="4">
+        <f>SUM(D331:R331)</f>
+        <v>102</v>
+      </c>
+      <c r="D331" s="3">
+        <v>11</v>
+      </c>
+      <c r="E331" s="3">
+        <v>21</v>
+      </c>
+      <c r="F331" s="3">
+        <v>32</v>
+      </c>
+      <c r="G331" s="3">
+        <v>19</v>
+      </c>
+      <c r="H331" s="3">
+        <v>19</v>
+      </c>
+      <c r="I331" s="3"/>
+      <c r="J331" s="3"/>
+      <c r="K331" s="3"/>
+      <c r="L331" s="3"/>
+      <c r="M331" s="3"/>
+      <c r="N331" s="3"/>
+      <c r="O331" s="3"/>
+      <c r="P331" s="3"/>
+      <c r="Q331" s="3"/>
+      <c r="R331" s="3"/>
+      <c r="S331" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="332" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A332" s="1">
+        <v>45488</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C332" s="4">
+        <f>SUM(D332:R332)</f>
+        <v>52</v>
+      </c>
+      <c r="D332" s="3">
+        <v>23</v>
+      </c>
+      <c r="E332" s="3">
+        <v>3</v>
+      </c>
+      <c r="F332" s="3">
+        <v>11</v>
+      </c>
+      <c r="G332" s="3">
+        <v>15</v>
+      </c>
+      <c r="H332" s="3"/>
+      <c r="I332" s="3"/>
+      <c r="J332" s="3"/>
+      <c r="K332" s="3"/>
+      <c r="L332" s="3"/>
+      <c r="M332" s="3"/>
+      <c r="N332" s="3"/>
+      <c r="O332" s="3"/>
+      <c r="P332" s="3"/>
+      <c r="Q332" s="3"/>
+      <c r="R332" s="3"/>
+      <c r="S332" s="13">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C338" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -13183,7 +13548,7 @@
       </c>
       <c r="B2" s="10">
         <f>SUM(Tabla2[Total])/(B4-B3+1)</f>
-        <v>25.615853658536587</v>
+        <v>26.642570281124499</v>
       </c>
       <c r="C2" s="10">
         <f>SUMIF(Tiempos!$S:$S,C1,Tiempos!$C:$C)/(C4-C3+1)</f>
@@ -13191,7 +13556,7 @@
       </c>
       <c r="D2" s="10">
         <f>SUMIF(Tiempos!$S:$S,D1,Tiempos!$C:$C)/(D4-D3+1)</f>
-        <v>42.031413612565444</v>
+        <v>44.126903553299492</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -13216,14 +13581,14 @@
       </c>
       <c r="B4" s="11">
         <f>MAX(Tabla2[Fecha])</f>
-        <v>45482</v>
+        <v>45488</v>
       </c>
       <c r="C4" s="11">
         <v>45291</v>
       </c>
       <c r="D4" s="11">
         <f>MAX(Tabla2[Fecha])</f>
-        <v>45482</v>
+        <v>45488</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -13263,11 +13628,11 @@
       </c>
       <c r="D10">
         <f>(D4-D3+1)*D2</f>
-        <v>8028</v>
+        <v>8693</v>
       </c>
       <c r="F10">
         <f>ROUND(D10*F9/D9,0)</f>
-        <v>267</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -13276,7 +13641,7 @@
       </c>
       <c r="D11" s="16">
         <f>D10/D9</f>
-        <v>0.73114754098360657</v>
+        <v>0.79171220400728592</v>
       </c>
     </row>
   </sheetData>
@@ -13287,10 +13652,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E9BC95-BDDC-4BA0-8C32-B1D087D6F575}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13355,26 +13720,31 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
curso de symfony 7
</commit_message>
<xml_diff>
--- a/00soportes/Tiempos.xlsx
+++ b/00soportes/Tiempos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\petrix\projects\cvpetrix2022\00soportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9558D7-22A0-415F-AFFA-4CB650767872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D6334-12C0-4808-BC15-1BB63E1F10B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7428" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="248">
   <si>
     <t>Fecha</t>
   </si>
@@ -1190,8 +1190,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:S841" totalsRowShown="0">
-  <autoFilter ref="A1:S841" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:S843" totalsRowShown="0">
+  <autoFilter ref="A1:S843" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="18">
       <filters>
         <filter val="2025"/>
@@ -1498,13 +1498,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y841"/>
+  <dimension ref="A1:Y843"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D829" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D832" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M845" sqref="M845"/>
+      <selection pane="bottomRight" activeCell="E844" sqref="E844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -1582,15 +1582,15 @@
       </c>
       <c r="V1" s="32">
         <f>Resumen!H2</f>
-        <v>30.135693215339234</v>
+        <v>30.020467836257311</v>
       </c>
       <c r="W1" s="33">
         <f>Resumen!D11</f>
-        <v>0.93296803652968041</v>
+        <v>0.93762557077625575</v>
       </c>
       <c r="X1" s="34">
         <f>Resumen!D7+Resumen!F10</f>
-        <v>45998</v>
+        <v>45999</v>
       </c>
     </row>
     <row r="2" spans="1:24" hidden="1">
@@ -32933,7 +32933,7 @@
         <v>31</v>
       </c>
       <c r="C836" s="29">
-        <f>SUM(D836:R836)</f>
+        <f t="shared" ref="C836:C841" si="18">SUM(D836:R836)</f>
         <v>29</v>
       </c>
       <c r="D836" s="30">
@@ -32968,7 +32968,7 @@
         <v>59</v>
       </c>
       <c r="C837" s="29">
-        <f>SUM(D837:R837)</f>
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
       <c r="D837" s="30">
@@ -33005,7 +33005,7 @@
         <v>59</v>
       </c>
       <c r="C838" s="29">
-        <f>SUM(D838:R838)</f>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="D838" s="30">
@@ -33048,7 +33048,7 @@
         <v>34</v>
       </c>
       <c r="C839" s="29">
-        <f>SUM(D839:R839)</f>
+        <f t="shared" si="18"/>
         <v>26</v>
       </c>
       <c r="D839" s="30">
@@ -33093,7 +33093,7 @@
         <v>59</v>
       </c>
       <c r="C840" s="29">
-        <f>SUM(D840:R840)</f>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="D840" s="30">
@@ -33130,7 +33130,7 @@
         <v>41</v>
       </c>
       <c r="C841" s="29">
-        <f>SUM(D841:R841)</f>
+        <f t="shared" si="18"/>
         <v>44</v>
       </c>
       <c r="D841" s="30">
@@ -33169,6 +33169,82 @@
       <c r="Q841" s="30"/>
       <c r="R841" s="30"/>
       <c r="S841" s="28">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="842" spans="1:19">
+      <c r="A842" s="27">
+        <v>45997</v>
+      </c>
+      <c r="B842" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C842" s="29">
+        <f>SUM(D842:R842)</f>
+        <v>33</v>
+      </c>
+      <c r="D842" s="30">
+        <v>7</v>
+      </c>
+      <c r="E842" s="30">
+        <v>8</v>
+      </c>
+      <c r="F842" s="30">
+        <v>6</v>
+      </c>
+      <c r="G842" s="30">
+        <v>11</v>
+      </c>
+      <c r="H842" s="30">
+        <v>1</v>
+      </c>
+      <c r="I842" s="30"/>
+      <c r="J842" s="30"/>
+      <c r="K842" s="30"/>
+      <c r="L842" s="30"/>
+      <c r="M842" s="30"/>
+      <c r="N842" s="30"/>
+      <c r="O842" s="30"/>
+      <c r="P842" s="30"/>
+      <c r="Q842" s="30"/>
+      <c r="R842" s="30"/>
+      <c r="S842" s="28">
+        <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="843" spans="1:19">
+      <c r="A843" s="27">
+        <v>45999</v>
+      </c>
+      <c r="B843" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C843" s="29">
+        <f>SUM(D843:R843)</f>
+        <v>18</v>
+      </c>
+      <c r="D843" s="30">
+        <v>17</v>
+      </c>
+      <c r="E843" s="30">
+        <v>1</v>
+      </c>
+      <c r="F843" s="30"/>
+      <c r="G843" s="30"/>
+      <c r="H843" s="30"/>
+      <c r="I843" s="30"/>
+      <c r="J843" s="30"/>
+      <c r="K843" s="30"/>
+      <c r="L843" s="30"/>
+      <c r="M843" s="30"/>
+      <c r="N843" s="30"/>
+      <c r="O843" s="30"/>
+      <c r="P843" s="30"/>
+      <c r="Q843" s="30"/>
+      <c r="R843" s="30"/>
+      <c r="S843" s="28">
         <f>YEAR(Tabla2[[#This Row],[Fecha]])</f>
         <v>2025</v>
       </c>
@@ -33539,7 +33615,7 @@
       </c>
       <c r="B2" s="25">
         <f>SUM(Tabla2[Total])/(B4-B3+1)</f>
-        <v>44.019704433497537</v>
+        <v>43.979832759468763</v>
       </c>
       <c r="C2" s="25">
         <f>SUMIF(Tiempos!$S:$S,C1,Tiempos!$C:$C)/(C4-C3+1)</f>
@@ -33563,7 +33639,7 @@
       </c>
       <c r="H2" s="25">
         <f>SUMIF(Tiempos!$S:$S,H1,Tiempos!$C:$C)/(H4-H3+1)</f>
-        <v>30.135693215339234</v>
+        <v>30.020467836257311</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -33602,7 +33678,7 @@
       </c>
       <c r="B4" s="26">
         <f>MAX(Tabla2[Fecha])</f>
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="C4" s="26">
         <v>44196</v>
@@ -33621,11 +33697,11 @@
       </c>
       <c r="H4" s="26">
         <f>MAX(Tabla2[Fecha])</f>
-        <v>45996</v>
+        <v>45999</v>
       </c>
       <c r="I4" s="26">
         <f>MAX(Tabla2[Fecha])</f>
-        <v>45996</v>
+        <v>45999</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -33665,11 +33741,11 @@
       </c>
       <c r="D10">
         <f>(H4-H3+1)*H2</f>
-        <v>10216</v>
+        <v>10267</v>
       </c>
       <c r="F10">
         <f>ROUND(D10*F9/D9,0)</f>
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -33678,7 +33754,7 @@
       </c>
       <c r="D11" s="19">
         <f>D10/D9</f>
-        <v>0.93296803652968041</v>
+        <v>0.93762557077625575</v>
       </c>
     </row>
   </sheetData>
@@ -34084,7 +34160,7 @@
       </c>
       <c r="B43" s="22">
         <f>SUMIF(Tiempos!B:B,A43,Tiempos!C:C)/60</f>
-        <v>8.7333333333333325</v>
+        <v>9.5833333333333339</v>
       </c>
     </row>
     <row r="44" spans="1:2">

</xml_diff>